<commit_message>
Fragezeichen in den weissen Bricks. Fragenkatalaog erweitert
</commit_message>
<xml_diff>
--- a/Neuer_Arzttarif_Frage_Antwort_Spiel.xlsx
+++ b/Neuer_Arzttarif_Frage_Antwort_Spiel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a5b72c7ff873d10/Dokumente/Private Projekte/Python/Brick/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5808CA80-7604-4CD0-87D6-6B215F64FE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{5808CA80-7604-4CD0-87D6-6B215F64FE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3324C737-D2A4-4E00-BC52-D6B8EF8223A3}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{A3D2235D-E1F2-41DB-828F-4F583D2A793C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="223">
   <si>
     <t>Stichwort</t>
   </si>
@@ -410,9 +410,6 @@
     <t>B) Durch die Typenbezeichnung "P".</t>
   </si>
   <si>
-    <t>C) Durch die Typenbezeichnung "L".</t>
-  </si>
-  <si>
     <t>Kostenneutrale Einführung</t>
   </si>
   <si>
@@ -449,9 +446,6 @@
     <t>Was müssen Ärztinnen und Ärzte sowie Einrichtungen und Spitäler unterzeichnen, um über TARDOC oder Ambulante Pauschalen abrechnen zu können?</t>
   </si>
   <si>
-    <t>A) Einen Einzelarbeitsvertrag mit der OAAT AG.</t>
-  </si>
-  <si>
     <t>B) Einen Vertrag mit der SASIS.</t>
   </si>
   <si>
@@ -464,9 +458,6 @@
     <t>Wo sind die Tarifkataloge für TARDOC und die Ambulanten Pauschalen als interaktive Version verfügbar?</t>
   </si>
   <si>
-    <t>A) Im Medreg.</t>
-  </si>
-  <si>
     <t>B) Im Tarifbrowser der OAAT AG.</t>
   </si>
   <si>
@@ -503,7 +494,217 @@
     <t>C) Nur für Leistungen in der Psychiatrie.</t>
   </si>
   <si>
-    <t>h</t>
+    <t>A) Einzelleistungstarif für ambulante ärztliche Leistungen in der Schweiz</t>
+  </si>
+  <si>
+    <t>A) Einen Einzelvertrag mit der OAAT AG.</t>
+  </si>
+  <si>
+    <t>A) Im MedReg.</t>
+  </si>
+  <si>
+    <t>C) Durch die Typenbezeichnung "N".</t>
+  </si>
+  <si>
+    <t>Mengenbeschränkung AA</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Ärztliche Konsultation, erste 5 Min.“ (AA.00.0010, Ärztliche Konsultation, erste 5 Min.) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Nur einmal pro Sitzung</t>
+  </si>
+  <si>
+    <t>Maximal dreimal pro Sitzung</t>
+  </si>
+  <si>
+    <t>Beliebig oft pro Sitzung</t>
+  </si>
+  <si>
+    <t>Kumulation AA</t>
+  </si>
+  <si>
+    <t>Können „Ärztliche Konsultation, erste 5 Min.“ (AA.00.0010, Ärztliche Konsultation, erste 5 Min.) und „Besuch, erste 5 Min.“ (AA.00.0030, Besuch, erste 5 Min.) zusammen abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Ja, immer</t>
+  </si>
+  <si>
+    <t>Nein, sie sind nicht kumulierbar</t>
+  </si>
+  <si>
+    <t>Nur an Wochenenden</t>
+  </si>
+  <si>
+    <t>Zuschlagregel AA</t>
+  </si>
+  <si>
+    <t>Unter welcher Voraussetzung darf „+ Ärztliche Konsultation, jede weitere 1 Min.“ (AA.00.0020, + Ärztliche Konsultation, jede weitere 1 Min.) abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Als eigenständige Leistung</t>
+  </si>
+  <si>
+    <t>Nur als Zuschlag zu AA.00.0010 (Ärztliche Konsultation, erste 5 Min.)</t>
+  </si>
+  <si>
+    <t>Bei jedem Folgetermin</t>
+  </si>
+  <si>
+    <t>Wie viele „+ Ärztliche Konsultation, jede weitere 1 Min.“ (AA.00.0020, + Ärztliche Konsultation, jede weitere 1 Min.) dürfen pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Maximal 15 pro Sitzung</t>
+  </si>
+  <si>
+    <t>Maximal 10 pro Sitzung</t>
+  </si>
+  <si>
+    <t>Ohne Begrenzung</t>
+  </si>
+  <si>
+    <t>Kumulation CA</t>
+  </si>
+  <si>
+    <t>Ist „Besuch, erste 5 Min.“ (AA.00.0030, Besuch, erste 5 Min.) kumulierbar mit „Notfallkonsultation am Telefon, erste 5 Min.“ (CA.15.0030, Notfallkonsultation am Telefon, erste 5 Min.)?</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Nein</t>
+  </si>
+  <si>
+    <t>Nur bei Hausärzten</t>
+  </si>
+  <si>
+    <t>Trigger Pauschalen</t>
+  </si>
+  <si>
+    <t>Wann wird die Pauschale „C00.10A“ (Stereotaktische Radiochirurgie: Gamma-Knife oder Bestrahlung v. Hirnmetastasen mit Anästhesie d. Anästhesist/in) ausgelöst?</t>
+  </si>
+  <si>
+    <t>Wenn bestimmte Einzelleistungen zusammen auftreten</t>
+  </si>
+  <si>
+    <t>Bei jeder Gamma-Knife-Therapie</t>
+  </si>
+  <si>
+    <t>Bei ambulanten Fällen mit Anästhesie</t>
+  </si>
+  <si>
+    <t>Können AA.00.0010 (Ärztliche Konsultation, erste 5 Min.) und AA.10.0010 (Telemedizinische Konsultation, erste 5 Min.) gemeinsam abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Ja, wenn verschiedene Ärzte beteiligt sind</t>
+  </si>
+  <si>
+    <t>Nur bei besonderen Notfällen</t>
+  </si>
+  <si>
+    <t>Wie oft darf „Besuch, erste 5 Min.“ (AA.00.0030, Besuch, erste 5 Min.) pro Sitzung verrechnet werden?</t>
+  </si>
+  <si>
+    <t>Maximal viermal pro Sitzung</t>
+  </si>
+  <si>
+    <t>Keine Begrenzung</t>
+  </si>
+  <si>
+    <t>Abrechnungsregel Wegzeit</t>
+  </si>
+  <si>
+    <t>Wann ist die Wegzeit (AA.00.0050, Wegzeit, pro 1 Min.) für einen erfolglosen Hausbesuch abrechenbar?</t>
+  </si>
+  <si>
+    <t>Immer, wenn der Patient nicht angetroffen wurde</t>
+  </si>
+  <si>
+    <t>Nur wenn die Abwesenheit medizinisch begründbar war</t>
+  </si>
+  <si>
+    <t>Nie, Wegzeit ist nur bei erfolgreichem Besuch erlaubt</t>
+  </si>
+  <si>
+    <t>Wie wird die Wegzeit (AA.00.0050, Wegzeit, pro 1 Min.) bei mehreren Patienten in einer Besuchstour abgerechnet?</t>
+  </si>
+  <si>
+    <t>Die gesamte Tour kann abgerechnet werden</t>
+  </si>
+  <si>
+    <t>Nur die Zeit zwischen zwei Patienten darf abgerechnet werden</t>
+  </si>
+  <si>
+    <t>Wegzeit ist hier nicht abrechenbar</t>
+  </si>
+  <si>
+    <t>Konsilium</t>
+  </si>
+  <si>
+    <t>Welche Leistungen sind in einem Konsilium (AA.00.0080, Ärztliches Konsilium, pro 1 Min.) inkludiert?</t>
+  </si>
+  <si>
+    <t>Nur die Beratung des Patienten</t>
+  </si>
+  <si>
+    <t>Beratung, Befragung, Studium der Akten, Dokumentation und schriftlicher Bericht</t>
+  </si>
+  <si>
+    <t>Nur das Schreiben eines Berichts</t>
+  </si>
+  <si>
+    <t>Wer darf ein Konsilium (AA.00.0080, Ärztliches Konsilium, pro 1 Min.) abrechnen?</t>
+  </si>
+  <si>
+    <t>Jeder Arzt</t>
+  </si>
+  <si>
+    <t>Nur Fachärzte mit spezieller Qualifikation</t>
+  </si>
+  <si>
+    <t>Nur der Hausarzt</t>
+  </si>
+  <si>
+    <t>Versicherungsauftrag</t>
+  </si>
+  <si>
+    <t>Dürfen Leistungen im Auftrag des Versicherers über AA.00.0010 (Ärztliche Konsultation, erste 5 Min.) abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Nein, hierfür ist AA.15.0090 (Leistung im Auftrag des Versicherers) zu verwenden</t>
+  </si>
+  <si>
+    <t>Nur bei stationären Aufenthalten</t>
+  </si>
+  <si>
+    <t>Telemedizin AA</t>
+  </si>
+  <si>
+    <t>Welche Tarifpositionen sind für telemedizinische Grundleistungen im Kapitel AA vorgesehen?</t>
+  </si>
+  <si>
+    <t>AA.10.0010 bis AA.10.0030 (Telemedizinische Grundleistungen)</t>
+  </si>
+  <si>
+    <t>AA.00.0010 bis AA.00.0040 (Konsultationen und Besuche)</t>
+  </si>
+  <si>
+    <t>Nur AA.00.0010 (Konsultation, erste 5 Min.)</t>
+  </si>
+  <si>
+    <t>Vor-/Nachbesprechung</t>
+  </si>
+  <si>
+    <t>Wie wird die Vor- und Nachbesprechung diagnostischer/therapeutischer Eingriffe mit Patienten (AA.00.0060, Vor- und Nachbesprechung, pro 1 Min.) abgerechnet?</t>
+  </si>
+  <si>
+    <t>Pro begonnene 10 Minuten</t>
+  </si>
+  <si>
+    <t>Pro Minute, max. 20 Minuten pro Sitzung</t>
+  </si>
+  <si>
+    <t>Pro Sitzung, pauschal</t>
   </si>
 </sst>
 </file>
@@ -629,13 +830,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22D44863-CD69-4320-B81B-9C0875E13C5F}" name="Tabelle1" displayName="Tabelle1" ref="A1:F31" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F31" xr:uid="{22D44863-CD69-4320-B81B-9C0875E13C5F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22D44863-CD69-4320-B81B-9C0875E13C5F}" name="Tabelle1" displayName="Tabelle1" ref="A1:F80" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F80" xr:uid="{22D44863-CD69-4320-B81B-9C0875E13C5F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{BD3B3692-3834-49BB-9097-73724DD1A58A}" name="Stichwort" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{906A98C3-8D52-477A-B9A0-CDC4D616F581}" name="Frage" dataDxfId="4"/>
@@ -965,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31FC0AD-4A42-4F5D-871F-F4892F5A15C7}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1007,7 +1204,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -1473,7 +1670,7 @@
         <v>123</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="F25" s="1">
         <v>2</v>
@@ -1481,19 +1678,19 @@
     </row>
     <row r="26" spans="1:6" ht="43" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="F26" s="1">
         <v>2</v>
@@ -1501,19 +1698,19 @@
     </row>
     <row r="27" spans="1:6" ht="43" x14ac:dyDescent="0.5">
       <c r="A27" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="F27" s="1">
         <v>2</v>
@@ -1521,19 +1718,19 @@
     </row>
     <row r="28" spans="1:6" ht="43" x14ac:dyDescent="0.5">
       <c r="A28" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="F28" s="1">
         <v>3</v>
@@ -1541,19 +1738,19 @@
     </row>
     <row r="29" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A29" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="F29" s="1">
         <v>2</v>
@@ -1561,19 +1758,19 @@
     </row>
     <row r="30" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A30" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="F30" s="1">
         <v>2</v>
@@ -1581,21 +1778,1001 @@
     </row>
     <row r="31" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="F31" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A32" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="A33" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F33" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A34" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A35" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A36" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F36" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A37" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A38" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F38" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A39" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A40" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F40" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A41" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F41" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A42" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F42" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A43" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A44" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F44" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A45" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="A46" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F46" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A47" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A48" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A49" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A50" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F50" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A51" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A52" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A53" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A54" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A55" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F55" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A56" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F56" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A57" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F57" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A58" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F58" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A59" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A60" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A61" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F61" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A62" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F62" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A63" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F63" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A64" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F64" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A65" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A66" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F66" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A67" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A68" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F68" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A69" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F69" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A70" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F70" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A71" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F71" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A72" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="A73" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F73" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A74" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F74" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A75" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F75" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A76" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F76" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A77" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A78" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F78" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A79" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F79" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+      <c r="A80" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F80" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Einige Fehler sind noch in game.js zu beheben
</commit_message>
<xml_diff>
--- a/Neuer_Arzttarif_Frage_Antwort_Spiel.xlsx
+++ b/Neuer_Arzttarif_Frage_Antwort_Spiel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a5b72c7ff873d10/Dokumente/Private Projekte/Python/Brick/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{5808CA80-7604-4CD0-87D6-6B215F64FE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3324C737-D2A4-4E00-BC52-D6B8EF8223A3}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{5808CA80-7604-4CD0-87D6-6B215F64FE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8610EE1-32B8-4D79-A0A1-03003FF084B6}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{A3D2235D-E1F2-41DB-828F-4F583D2A793C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="320">
   <si>
     <t>Stichwort</t>
   </si>
@@ -705,6 +705,297 @@
   </si>
   <si>
     <t>Pro Sitzung, pauschal</t>
+  </si>
+  <si>
+    <t>Definition Einzelleistung</t>
+  </si>
+  <si>
+    <t>Was ist eine Einzelleistung im TARDOC?</t>
+  </si>
+  <si>
+    <t>Eine einzelne, genau definierte abrechenbare medizinische Handlung</t>
+  </si>
+  <si>
+    <t>Ein Bündel von Einzelleistungen</t>
+  </si>
+  <si>
+    <t>Eine spezielle Form der Pauschale</t>
+  </si>
+  <si>
+    <t>Kumulationsverbot</t>
+  </si>
+  <si>
+    <t>Was bedeutet ein Kumulationsverbot bei zwei TARDOC-Leistungen?</t>
+  </si>
+  <si>
+    <t>Sie dürfen nicht in derselben Sitzung abgerechnet werden</t>
+  </si>
+  <si>
+    <t>Sie müssen gemeinsam abgerechnet werden</t>
+  </si>
+  <si>
+    <t>Sie gelten nur im Spital</t>
+  </si>
+  <si>
+    <t>Dignität</t>
+  </si>
+  <si>
+    <t>Wo findet man die für eine Leistung vorgeschriebene Dignität im Katalog?</t>
+  </si>
+  <si>
+    <t>Direkt in der Leistungstabelle, bei jeder Tarifposition</t>
+  </si>
+  <si>
+    <t>Nur im Anhang</t>
+  </si>
+  <si>
+    <t>Auf der Rechnung</t>
+  </si>
+  <si>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t>Was ist ein typischer "Trigger" für eine ambulante Pauschale?</t>
+  </si>
+  <si>
+    <t>Das gleichzeitige Vorliegen mehrerer vordefinierter Einzelleistungen</t>
+  </si>
+  <si>
+    <t>Die Unterschrift des Arztes</t>
+  </si>
+  <si>
+    <t>Die Abgabe eines Medikaments</t>
+  </si>
+  <si>
+    <t>Definition Pauschale</t>
+  </si>
+  <si>
+    <t>Was ist eine Pauschale laut TARDOC?</t>
+  </si>
+  <si>
+    <t>Eine abgerechnete Kombination medizinisch sinnvoll zusammengefasster Leistungen</t>
+  </si>
+  <si>
+    <t>Eine frei wählbare Abrechnungseinheit</t>
+  </si>
+  <si>
+    <t>Eine doppelt so hohe Einzelleistung</t>
+  </si>
+  <si>
+    <t>Mengenbegrenzung</t>
+  </si>
+  <si>
+    <t>Wie oft darf eine telemedizinische Konsultation (AA.10.0010, Telemedizinische Konsultation, erste 5 Min.) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Maximal einmal pro Sitzung</t>
+  </si>
+  <si>
+    <t>Maximal zweimal</t>
+  </si>
+  <si>
+    <t>Beliebig oft</t>
+  </si>
+  <si>
+    <t>Telemedizin</t>
+  </si>
+  <si>
+    <t>Was unterscheidet die telemedizinische Konsultation (AA.10.0010) von der Präsenz-Konsultation?</t>
+  </si>
+  <si>
+    <t>Sie darf nicht zusammen mit AA.00.0010 (Konsultation, erste 5 Min.) abgerechnet werden</t>
+  </si>
+  <si>
+    <t>Sie ist immer günstiger</t>
+  </si>
+  <si>
+    <t>Sie braucht keine Dokumentation</t>
+  </si>
+  <si>
+    <t>Kumulation</t>
+  </si>
+  <si>
+    <t>Können AA.00.0030 (Besuch, erste 5 Min.) und AA.00.0010 (Konsultation, erste 5 Min.) in derselben Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Nein, ein Kumulationsverbot besteht</t>
+  </si>
+  <si>
+    <t>Ja, wenn sie am gleichen Tag stattfinden</t>
+  </si>
+  <si>
+    <t>Nur bei unterschiedlichen Diagnosen</t>
+  </si>
+  <si>
+    <t>Wegzeit</t>
+  </si>
+  <si>
+    <t>Wann darf Wegzeit (AA.00.0050, Wegzeit, pro 1 Min.) abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Nur bei ärztlichen Hausbesuchen außerhalb der Praxis</t>
+  </si>
+  <si>
+    <t>Bei jedem Praxisbesuch</t>
+  </si>
+  <si>
+    <t>Nie</t>
+  </si>
+  <si>
+    <t>Pauschaleninhalt</t>
+  </si>
+  <si>
+    <t>Was ist in den meisten ambulanten Pauschalen (z.B. C00.10A) zusätzlich zu den Hauptleistungen enthalten?</t>
+  </si>
+  <si>
+    <t>Gewisse diagnostische Einzelleistungen und bestimmte Grundpflege</t>
+  </si>
+  <si>
+    <t>Alle Medikamente</t>
+  </si>
+  <si>
+    <t>Nur ärztliche Zeit</t>
+  </si>
+  <si>
+    <t>Pauschalenprüfung</t>
+  </si>
+  <si>
+    <t>Wie erkennt das System, ob eine Pauschale ausgelöst wird?</t>
+  </si>
+  <si>
+    <t>Durch die technische Prüflogik im Katalog (Triggerregeln und Mindestleistungen)</t>
+  </si>
+  <si>
+    <t>Durch Handaufschreiben</t>
+  </si>
+  <si>
+    <t>Per Zufall</t>
+  </si>
+  <si>
+    <t>Hausarzt-Notfall</t>
+  </si>
+  <si>
+    <t>Welche Voraussetzung braucht es für CA.15.0030 (Notfallkonsultation am Telefon, erste 5 Min.)?</t>
+  </si>
+  <si>
+    <t>Akute, nicht planbare gesundheitliche Situation</t>
+  </si>
+  <si>
+    <t>Jedes Symptom</t>
+  </si>
+  <si>
+    <t>Vorherige Konsultation</t>
+  </si>
+  <si>
+    <t>Hausbesuch</t>
+  </si>
+  <si>
+    <t>Was gilt als Hausbesuch im Kapitel CA?</t>
+  </si>
+  <si>
+    <t>Persönliche ärztliche Behandlung außerhalb der Praxis</t>
+  </si>
+  <si>
+    <t>Telefonischer Kontakt</t>
+  </si>
+  <si>
+    <t>Behandlung im Spital</t>
+  </si>
+  <si>
+    <t>Zuschläge</t>
+  </si>
+  <si>
+    <t>Wann darf der Zuschlag AA.00.0040 (+ Besuch, jede weitere 1 Min.) abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Nur als Ergänzung zu AA.00.0030 (Besuch, erste 5 Min.)</t>
+  </si>
+  <si>
+    <t>Immer, unabhängig von anderen Leistungen</t>
+  </si>
+  <si>
+    <t>Bei jedem Patienten</t>
+  </si>
+  <si>
+    <t>Einzelleistung in Pauschale</t>
+  </si>
+  <si>
+    <t>Was passiert mit Einzelleistungen, die im Gültigkeitsbereich einer Pauschale erbracht werden?</t>
+  </si>
+  <si>
+    <t>Sie sind in der Pauschale abgegolten und nicht separat abrechnungsfähig</t>
+  </si>
+  <si>
+    <t>Sie müssen immer separat abgerechnet werden</t>
+  </si>
+  <si>
+    <t>Sie gelten doppelt</t>
+  </si>
+  <si>
+    <t>Kombinierbarkeit Pauschale</t>
+  </si>
+  <si>
+    <t>Können zwei ambulante Pauschalen für die gleiche Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Nur, wenn beide unterschiedliche Leistungsbereiche abdecken und kein Kumulationsverbot besteht</t>
+  </si>
+  <si>
+    <t>Immer</t>
+  </si>
+  <si>
+    <t>Dokumentation</t>
+  </si>
+  <si>
+    <t>Was ist bei der Abrechnung jeder Pauschale zwingend erforderlich?</t>
+  </si>
+  <si>
+    <t>Die lückenlose Dokumentation der erbrachten Einzelleistungen und Begründungen</t>
+  </si>
+  <si>
+    <t>Nur der Name des Patienten</t>
+  </si>
+  <si>
+    <t>Die Höhe der Vergütung</t>
+  </si>
+  <si>
+    <t>Auslösung Pauschale</t>
+  </si>
+  <si>
+    <t>Wer löst die Pauschale technisch aus?</t>
+  </si>
+  <si>
+    <t>Das Abrechnungssystem/Grouper anhand der hinterlegten Trigger</t>
+  </si>
+  <si>
+    <t>Der Patient selbst</t>
+  </si>
+  <si>
+    <t>Der Chefarzt</t>
+  </si>
+  <si>
+    <t>Kombinierbarkeit AA/CA</t>
+  </si>
+  <si>
+    <t>Dürfen Leistungen aus Kapitel AA und CA kombiniert abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Nur, wenn kein Kumulationsverbot besteht</t>
+  </si>
+  <si>
+    <t>Leistungsbeschreibung</t>
+  </si>
+  <si>
+    <t>Wo findet man die Beschreibung einer Pauschale wie C00.20A?</t>
+  </si>
+  <si>
+    <t>Im Leistungskatalog (z.B. TARDOC/AMBULANT), direkt neben dem Pauschalencode</t>
+  </si>
+  <si>
+    <t>Nur auf der Rechnung</t>
+  </si>
+  <si>
+    <t>Nur beim Versicherer</t>
   </si>
 </sst>
 </file>
@@ -748,11 +1039,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -830,9 +1118,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22D44863-CD69-4320-B81B-9C0875E13C5F}" name="Tabelle1" displayName="Tabelle1" ref="A1:F80" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F80" xr:uid="{22D44863-CD69-4320-B81B-9C0875E13C5F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22D44863-CD69-4320-B81B-9C0875E13C5F}" name="Tabelle1" displayName="Tabelle1" ref="A1:F96" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F96" xr:uid="{22D44863-CD69-4320-B81B-9C0875E13C5F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{BD3B3692-3834-49BB-9097-73724DD1A58A}" name="Stichwort" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{906A98C3-8D52-477A-B9A0-CDC4D616F581}" name="Frage" dataDxfId="4"/>
@@ -1162,1618 +1454,1938 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31FC0AD-4A42-4F5D-871F-F4892F5A15C7}">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.76171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.234375" customWidth="1"/>
-    <col min="3" max="5" width="38.234375" customWidth="1"/>
+    <col min="1" max="1" width="19.05859375" customWidth="1"/>
+    <col min="2" max="2" width="44.41015625" customWidth="1"/>
+    <col min="3" max="5" width="45.703125" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>152</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A3" s="2" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A4" s="2" t="s">
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A5" s="2" t="s">
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A6" s="2" t="s">
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A8" s="2" t="s">
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A9" s="2" t="s">
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A10" s="2" t="s">
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="71.7" x14ac:dyDescent="0.5">
-      <c r="A11" s="2" t="s">
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A12" s="2" t="s">
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="71.7" x14ac:dyDescent="0.5">
-      <c r="A13" s="2" t="s">
+      <c r="F12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="100.35" x14ac:dyDescent="0.5">
-      <c r="A14" s="2" t="s">
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A15" s="2" t="s">
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A16" s="2" t="s">
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A17" s="2" t="s">
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>84</v>
       </c>
-      <c r="F17" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A18" s="2" t="s">
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="71.7" x14ac:dyDescent="0.5">
-      <c r="A19" s="2" t="s">
+      <c r="F18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>93</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>94</v>
       </c>
-      <c r="F19" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A20" s="2" t="s">
+      <c r="F19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>99</v>
       </c>
-      <c r="F20" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A21" s="2" t="s">
+      <c r="F20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>104</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>108</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>109</v>
       </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A23" s="2" t="s">
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A23" t="s">
         <v>110</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>113</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A24" s="2" t="s">
+      <c r="F23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>116</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>117</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>118</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>119</v>
       </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A25" s="2" t="s">
+      <c r="F24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
         <v>120</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>121</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>122</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>123</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>155</v>
       </c>
-      <c r="F25" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A26" s="2" t="s">
+      <c r="F25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
         <v>124</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>126</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>127</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>128</v>
       </c>
-      <c r="F26" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A27" s="2" t="s">
+      <c r="F26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
         <v>129</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>130</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>131</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>132</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>133</v>
       </c>
-      <c r="F27" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A28" s="2" t="s">
+      <c r="F27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
         <v>134</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>135</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>153</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>136</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>137</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
         <v>138</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>139</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>154</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>140</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>141</v>
       </c>
-      <c r="F29" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A30" s="2" t="s">
+      <c r="F29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A30" t="s">
         <v>142</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>143</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>145</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>146</v>
       </c>
-      <c r="F30" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A31" s="2" t="s">
+      <c r="F30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A31" t="s">
         <v>147</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>148</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>149</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>150</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>151</v>
       </c>
-      <c r="F31" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A32" s="2" t="s">
+      <c r="F31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
         <v>156</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>157</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>159</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>160</v>
       </c>
-      <c r="F32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A33" s="2" t="s">
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A33" t="s">
         <v>161</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>162</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>163</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>164</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>165</v>
       </c>
-      <c r="F33" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A34" s="2" t="s">
+      <c r="F33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
         <v>166</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>167</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>168</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>169</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>170</v>
       </c>
-      <c r="F34" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A35" s="2" t="s">
+      <c r="F34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
         <v>156</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>171</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>172</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>173</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>174</v>
       </c>
-      <c r="F35" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A36" s="2" t="s">
+      <c r="F35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
         <v>175</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>176</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>177</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" t="s">
         <v>178</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>179</v>
       </c>
-      <c r="F36" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A37" s="2" t="s">
+      <c r="F36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
         <v>180</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>181</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>182</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" t="s">
         <v>183</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>184</v>
       </c>
-      <c r="F37" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A38" s="2" t="s">
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
         <v>161</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>185</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>186</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" t="s">
         <v>164</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>187</v>
       </c>
-      <c r="F38" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A39" s="2" t="s">
+      <c r="F38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A39" t="s">
         <v>156</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>188</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>158</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" t="s">
         <v>189</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>190</v>
       </c>
-      <c r="F39" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A40" s="2" t="s">
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A40" t="s">
         <v>191</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>192</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>193</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" t="s">
         <v>194</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>195</v>
       </c>
-      <c r="F40" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A41" s="2" t="s">
+      <c r="F40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A41" t="s">
         <v>191</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>196</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>197</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" t="s">
         <v>198</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>199</v>
       </c>
-      <c r="F41" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A42" s="2" t="s">
+      <c r="F41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A42" t="s">
         <v>200</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>201</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>202</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" t="s">
         <v>203</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>204</v>
       </c>
-      <c r="F42" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A43" s="2" t="s">
+      <c r="F42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A43" t="s">
         <v>200</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>205</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>206</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" t="s">
         <v>207</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>208</v>
       </c>
-      <c r="F43" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A44" s="2" t="s">
+      <c r="F43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A44" t="s">
         <v>209</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>210</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>163</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" t="s">
         <v>211</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>212</v>
       </c>
-      <c r="F44" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A45" s="2" t="s">
+      <c r="F44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A45" t="s">
         <v>213</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>214</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" t="s">
         <v>215</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" t="s">
         <v>216</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>217</v>
       </c>
-      <c r="F45" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A46" s="2" t="s">
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A46" t="s">
         <v>218</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>219</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
         <v>220</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" t="s">
         <v>221</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>222</v>
       </c>
-      <c r="F46" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A47" s="2" t="s">
+      <c r="F46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A47" t="s">
         <v>180</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>181</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" t="s">
         <v>182</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" t="s">
         <v>183</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>184</v>
       </c>
-      <c r="F47" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A48" s="2" t="s">
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A48" t="s">
         <v>156</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>157</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" t="s">
         <v>158</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" t="s">
         <v>159</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" t="s">
         <v>160</v>
       </c>
-      <c r="F48" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A49" s="2" t="s">
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A49" t="s">
         <v>213</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>214</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" t="s">
         <v>215</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" t="s">
         <v>216</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>217</v>
       </c>
-      <c r="F49" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A50" s="2" t="s">
+      <c r="F49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A50" t="s">
         <v>200</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>201</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" t="s">
         <v>202</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" t="s">
         <v>203</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" t="s">
         <v>204</v>
       </c>
-      <c r="F50" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A51" s="2" t="s">
+      <c r="F50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A51" t="s">
         <v>156</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>157</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" t="s">
         <v>158</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" t="s">
         <v>159</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" t="s">
         <v>160</v>
       </c>
-      <c r="F51" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A52" s="2" t="s">
+      <c r="F51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A52" t="s">
         <v>213</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>214</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
         <v>215</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" t="s">
         <v>216</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" t="s">
         <v>217</v>
       </c>
-      <c r="F52" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A53" s="2" t="s">
+      <c r="F52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A53" t="s">
         <v>156</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>157</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" t="s">
         <v>158</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" t="s">
         <v>159</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" t="s">
         <v>160</v>
       </c>
-      <c r="F53" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A54" s="2" t="s">
+      <c r="F53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A54" t="s">
         <v>156</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>157</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" t="s">
         <v>158</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" t="s">
         <v>159</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" t="s">
         <v>160</v>
       </c>
-      <c r="F54" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A55" s="2" t="s">
+      <c r="F54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A55" t="s">
         <v>161</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>185</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" t="s">
         <v>186</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" t="s">
         <v>164</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" t="s">
         <v>187</v>
       </c>
-      <c r="F55" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A56" s="2" t="s">
+      <c r="F55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A56" t="s">
         <v>161</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>185</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" t="s">
         <v>186</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" t="s">
         <v>164</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" t="s">
         <v>187</v>
       </c>
-      <c r="F56" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A57" s="2" t="s">
+      <c r="F56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A57" t="s">
         <v>191</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>196</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" t="s">
         <v>197</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" t="s">
         <v>198</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" t="s">
         <v>199</v>
       </c>
-      <c r="F57" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A58" s="2" t="s">
+      <c r="F57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A58" t="s">
+        <v>156</v>
+      </c>
+      <c r="B58" t="s">
+        <v>188</v>
+      </c>
+      <c r="C58" t="s">
+        <v>158</v>
+      </c>
+      <c r="D58" t="s">
+        <v>189</v>
+      </c>
+      <c r="E58" t="s">
+        <v>190</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A59" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" t="s">
+        <v>157</v>
+      </c>
+      <c r="C59" t="s">
+        <v>158</v>
+      </c>
+      <c r="D59" t="s">
+        <v>159</v>
+      </c>
+      <c r="E59" t="s">
+        <v>160</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A60" t="s">
         <v>191</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B60" t="s">
         <v>196</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C60" t="s">
         <v>197</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D60" t="s">
         <v>198</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E60" t="s">
         <v>199</v>
       </c>
-      <c r="F58" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A59" s="2" t="s">
+      <c r="F60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A61" t="s">
+        <v>200</v>
+      </c>
+      <c r="B61" t="s">
+        <v>201</v>
+      </c>
+      <c r="C61" t="s">
+        <v>202</v>
+      </c>
+      <c r="D61" t="s">
+        <v>203</v>
+      </c>
+      <c r="E61" t="s">
+        <v>204</v>
+      </c>
+      <c r="F61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A62" t="s">
+        <v>161</v>
+      </c>
+      <c r="B62" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" t="s">
+        <v>186</v>
+      </c>
+      <c r="D62" t="s">
+        <v>164</v>
+      </c>
+      <c r="E62" t="s">
+        <v>187</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A63" t="s">
         <v>156</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B63" t="s">
+        <v>157</v>
+      </c>
+      <c r="C63" t="s">
+        <v>158</v>
+      </c>
+      <c r="D63" t="s">
+        <v>159</v>
+      </c>
+      <c r="E63" t="s">
+        <v>160</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A64" t="s">
+        <v>156</v>
+      </c>
+      <c r="B64" t="s">
+        <v>157</v>
+      </c>
+      <c r="C64" t="s">
+        <v>158</v>
+      </c>
+      <c r="D64" t="s">
+        <v>159</v>
+      </c>
+      <c r="E64" t="s">
+        <v>160</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A65" t="s">
+        <v>200</v>
+      </c>
+      <c r="B65" t="s">
+        <v>201</v>
+      </c>
+      <c r="C65" t="s">
+        <v>202</v>
+      </c>
+      <c r="D65" t="s">
+        <v>203</v>
+      </c>
+      <c r="E65" t="s">
+        <v>204</v>
+      </c>
+      <c r="F65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A66" t="s">
+        <v>156</v>
+      </c>
+      <c r="B66" t="s">
         <v>188</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C66" t="s">
         <v>158</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D66" t="s">
         <v>189</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E66" t="s">
         <v>190</v>
       </c>
-      <c r="F59" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A60" s="2" t="s">
+      <c r="F66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A67" t="s">
+        <v>166</v>
+      </c>
+      <c r="B67" t="s">
+        <v>167</v>
+      </c>
+      <c r="C67" t="s">
+        <v>168</v>
+      </c>
+      <c r="D67" t="s">
+        <v>169</v>
+      </c>
+      <c r="E67" t="s">
+        <v>170</v>
+      </c>
+      <c r="F67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A68" t="s">
         <v>156</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B68" t="s">
         <v>157</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C68" t="s">
         <v>158</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D68" t="s">
         <v>159</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E68" t="s">
         <v>160</v>
       </c>
-      <c r="F60" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A61" s="2" t="s">
+      <c r="F68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A69" t="s">
+        <v>218</v>
+      </c>
+      <c r="B69" t="s">
+        <v>219</v>
+      </c>
+      <c r="C69" t="s">
+        <v>220</v>
+      </c>
+      <c r="D69" t="s">
+        <v>221</v>
+      </c>
+      <c r="E69" t="s">
+        <v>222</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A70" t="s">
+        <v>180</v>
+      </c>
+      <c r="B70" t="s">
+        <v>181</v>
+      </c>
+      <c r="C70" t="s">
+        <v>182</v>
+      </c>
+      <c r="D70" t="s">
+        <v>183</v>
+      </c>
+      <c r="E70" t="s">
+        <v>184</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A71" t="s">
+        <v>200</v>
+      </c>
+      <c r="B71" t="s">
+        <v>201</v>
+      </c>
+      <c r="C71" t="s">
+        <v>202</v>
+      </c>
+      <c r="D71" t="s">
+        <v>203</v>
+      </c>
+      <c r="E71" t="s">
+        <v>204</v>
+      </c>
+      <c r="F71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A72" t="s">
+        <v>200</v>
+      </c>
+      <c r="B72" t="s">
+        <v>201</v>
+      </c>
+      <c r="C72" t="s">
+        <v>202</v>
+      </c>
+      <c r="D72" t="s">
+        <v>203</v>
+      </c>
+      <c r="E72" t="s">
+        <v>204</v>
+      </c>
+      <c r="F72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A73" t="s">
+        <v>156</v>
+      </c>
+      <c r="B73" t="s">
+        <v>157</v>
+      </c>
+      <c r="C73" t="s">
+        <v>158</v>
+      </c>
+      <c r="D73" t="s">
+        <v>159</v>
+      </c>
+      <c r="E73" t="s">
+        <v>160</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A74" t="s">
         <v>191</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B74" t="s">
+        <v>192</v>
+      </c>
+      <c r="C74" t="s">
+        <v>193</v>
+      </c>
+      <c r="D74" t="s">
+        <v>194</v>
+      </c>
+      <c r="E74" t="s">
+        <v>195</v>
+      </c>
+      <c r="F74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A75" t="s">
+        <v>191</v>
+      </c>
+      <c r="B75" t="s">
         <v>196</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C75" t="s">
         <v>197</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D75" t="s">
         <v>198</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E75" t="s">
         <v>199</v>
       </c>
-      <c r="F61" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A62" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F62" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A63" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F63" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A64" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F64" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A65" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F65" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A66" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F66" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A67" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F67" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A68" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F68" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A69" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F69" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A70" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F70" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A71" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F71" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A72" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F72" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A73" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F73" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A74" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F74" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A75" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F75" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A76" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F76" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A77" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F77" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A78" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="F78" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A79" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F79" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A80" s="2" t="s">
+      <c r="F75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A76" t="s">
         <v>175</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B76" t="s">
         <v>176</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C76" t="s">
         <v>177</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D76" t="s">
         <v>178</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E76" t="s">
         <v>179</v>
       </c>
-      <c r="F80" s="1">
-        <v>2</v>
+      <c r="F76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A77" t="s">
+        <v>223</v>
+      </c>
+      <c r="B77" t="s">
+        <v>224</v>
+      </c>
+      <c r="C77" t="s">
+        <v>225</v>
+      </c>
+      <c r="D77" t="s">
+        <v>226</v>
+      </c>
+      <c r="E77" t="s">
+        <v>227</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A78" t="s">
+        <v>228</v>
+      </c>
+      <c r="B78" t="s">
+        <v>229</v>
+      </c>
+      <c r="C78" t="s">
+        <v>230</v>
+      </c>
+      <c r="D78" t="s">
+        <v>231</v>
+      </c>
+      <c r="E78" t="s">
+        <v>232</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A79" t="s">
+        <v>233</v>
+      </c>
+      <c r="B79" t="s">
+        <v>234</v>
+      </c>
+      <c r="C79" t="s">
+        <v>235</v>
+      </c>
+      <c r="D79" t="s">
+        <v>236</v>
+      </c>
+      <c r="E79" t="s">
+        <v>237</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A80" t="s">
+        <v>238</v>
+      </c>
+      <c r="B80" t="s">
+        <v>239</v>
+      </c>
+      <c r="C80" t="s">
+        <v>240</v>
+      </c>
+      <c r="D80" t="s">
+        <v>241</v>
+      </c>
+      <c r="E80" t="s">
+        <v>242</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A81" t="s">
+        <v>243</v>
+      </c>
+      <c r="B81" t="s">
+        <v>244</v>
+      </c>
+      <c r="C81" t="s">
+        <v>245</v>
+      </c>
+      <c r="D81" t="s">
+        <v>246</v>
+      </c>
+      <c r="E81" t="s">
+        <v>247</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A82" t="s">
+        <v>248</v>
+      </c>
+      <c r="B82" t="s">
+        <v>249</v>
+      </c>
+      <c r="C82" t="s">
+        <v>250</v>
+      </c>
+      <c r="D82" t="s">
+        <v>251</v>
+      </c>
+      <c r="E82" t="s">
+        <v>252</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A83" t="s">
+        <v>253</v>
+      </c>
+      <c r="B83" t="s">
+        <v>254</v>
+      </c>
+      <c r="C83" t="s">
+        <v>255</v>
+      </c>
+      <c r="D83" t="s">
+        <v>256</v>
+      </c>
+      <c r="E83" t="s">
+        <v>257</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A84" t="s">
+        <v>258</v>
+      </c>
+      <c r="B84" t="s">
+        <v>259</v>
+      </c>
+      <c r="C84" t="s">
+        <v>260</v>
+      </c>
+      <c r="D84" t="s">
+        <v>261</v>
+      </c>
+      <c r="E84" t="s">
+        <v>262</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A85" t="s">
+        <v>263</v>
+      </c>
+      <c r="B85" t="s">
+        <v>264</v>
+      </c>
+      <c r="C85" t="s">
+        <v>265</v>
+      </c>
+      <c r="D85" t="s">
+        <v>266</v>
+      </c>
+      <c r="E85" t="s">
+        <v>267</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A86" t="s">
+        <v>268</v>
+      </c>
+      <c r="B86" t="s">
+        <v>269</v>
+      </c>
+      <c r="C86" t="s">
+        <v>270</v>
+      </c>
+      <c r="D86" t="s">
+        <v>271</v>
+      </c>
+      <c r="E86" t="s">
+        <v>272</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A87" t="s">
+        <v>273</v>
+      </c>
+      <c r="B87" t="s">
+        <v>274</v>
+      </c>
+      <c r="C87" t="s">
+        <v>275</v>
+      </c>
+      <c r="D87" t="s">
+        <v>276</v>
+      </c>
+      <c r="E87" t="s">
+        <v>277</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A88" t="s">
+        <v>278</v>
+      </c>
+      <c r="B88" t="s">
+        <v>279</v>
+      </c>
+      <c r="C88" t="s">
+        <v>280</v>
+      </c>
+      <c r="D88" t="s">
+        <v>281</v>
+      </c>
+      <c r="E88" t="s">
+        <v>282</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A89" t="s">
+        <v>283</v>
+      </c>
+      <c r="B89" t="s">
+        <v>284</v>
+      </c>
+      <c r="C89" t="s">
+        <v>285</v>
+      </c>
+      <c r="D89" t="s">
+        <v>286</v>
+      </c>
+      <c r="E89" t="s">
+        <v>287</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A90" t="s">
+        <v>288</v>
+      </c>
+      <c r="B90" t="s">
+        <v>289</v>
+      </c>
+      <c r="C90" t="s">
+        <v>290</v>
+      </c>
+      <c r="D90" t="s">
+        <v>291</v>
+      </c>
+      <c r="E90" t="s">
+        <v>292</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A91" t="s">
+        <v>293</v>
+      </c>
+      <c r="B91" t="s">
+        <v>294</v>
+      </c>
+      <c r="C91" t="s">
+        <v>295</v>
+      </c>
+      <c r="D91" t="s">
+        <v>296</v>
+      </c>
+      <c r="E91" t="s">
+        <v>297</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A92" t="s">
+        <v>298</v>
+      </c>
+      <c r="B92" t="s">
+        <v>299</v>
+      </c>
+      <c r="C92" t="s">
+        <v>300</v>
+      </c>
+      <c r="D92" t="s">
+        <v>301</v>
+      </c>
+      <c r="E92" t="s">
+        <v>267</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A93" t="s">
+        <v>302</v>
+      </c>
+      <c r="B93" t="s">
+        <v>303</v>
+      </c>
+      <c r="C93" t="s">
+        <v>304</v>
+      </c>
+      <c r="D93" t="s">
+        <v>305</v>
+      </c>
+      <c r="E93" t="s">
+        <v>306</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A94" t="s">
+        <v>307</v>
+      </c>
+      <c r="B94" t="s">
+        <v>308</v>
+      </c>
+      <c r="C94" t="s">
+        <v>309</v>
+      </c>
+      <c r="D94" t="s">
+        <v>310</v>
+      </c>
+      <c r="E94" t="s">
+        <v>311</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A95" t="s">
+        <v>312</v>
+      </c>
+      <c r="B95" t="s">
+        <v>313</v>
+      </c>
+      <c r="C95" t="s">
+        <v>314</v>
+      </c>
+      <c r="D95" t="s">
+        <v>301</v>
+      </c>
+      <c r="E95" t="s">
+        <v>267</v>
+      </c>
+      <c r="F95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A96" t="s">
+        <v>315</v>
+      </c>
+      <c r="B96" t="s">
+        <v>316</v>
+      </c>
+      <c r="C96" t="s">
+        <v>317</v>
+      </c>
+      <c r="D96" t="s">
+        <v>318</v>
+      </c>
+      <c r="E96" t="s">
+        <v>319</v>
+      </c>
+      <c r="F96">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Here's a summary of the changes: - I added a loading screen with the message 'Spiel und Quiz wird aufgestartet' that displays while assets are loading. - I implemented global ESC key functionality to hide the game container when no popups are active. - I ensured the existing ESC key behavior for quiz and game-end popups remains unchanged. You confirmed the ESC key functionality. The loading screen will need to be tested in the live environment.
</commit_message>
<xml_diff>
--- a/Neuer_Arzttarif_Frage_Antwort_Spiel.xlsx
+++ b/Neuer_Arzttarif_Frage_Antwort_Spiel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beata\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a5b72c7ff873d10/Dokumente/Private Projekte/Python/Brick/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE554369-1DEB-4A89-993D-DF665B0B90FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{CE554369-1DEB-4A89-993D-DF665B0B90FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8957EA5-2F95-429F-8510-7B72870A8CA9}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="475">
   <si>
     <t>Stichwort</t>
   </si>
@@ -550,156 +550,51 @@
     <t>Wo findet man die Beschreibung einer Pauschale wie C00.20A?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Ärztliche Konsultation, erste 5 Min." (LKN AA.00.0010) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Mit welcher Tarifposition darf die Leistung AA.00.0010 nicht kumuliert werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „+ Ärztliche Konsultation, jede weitere 1 Min." (LKN AA.00.0020) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Besuch, erste 5 Min." (LKN AA.00.0030) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Mit welcher Tarifposition darf die Leistung AA.00.0030 nicht kumuliert werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „+ Besuch, jede weitere 1 Min." (LKN AA.00.0040) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Wegzeit, pro 1 Min." (LKN AA.00.0050) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Vor-und Nachbesprechung diagnostischer/therapeutischer Eingriffe mit Patienten, pro 1 Min." (LKN AA.00.0060) pro tage abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Instruktion von Selbstmessungen und/oder Selbstbehandlungen durch den Arzt, pro 1 Min." (LKN AA.00.0070) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Instruktion von Selbstmessungen und/oder Selbstbehandlungen durch den Arzt, pro 1 Min." (LKN AA.00.0070) pro tage abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Ärztliches Konsilium, pro 1 Min." (LKN AA.00.0080) pro tage abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Mit welcher Tarifposition darf die Leistung AA.00.0080 nicht kumuliert werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Spezifische lmpfberatung bei franchisebefreiten lmpfungen, pro 1 Min." (LKN AA.00.0090) pro tage abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Mit welcher Tarifposition darf die Leistung AA.00.0090 nicht kumuliert werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Kreislauf" (LKN AA.05.0010) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Augen" (LKN AA.05.0020) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Ohren" (LKN AA.05.0030) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Luftwege" (LKN AA.05.0040) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Wirbelsäule" (LKN AA.05.0050) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Abdomen" (LKN AA.05.0060) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Uro-Genital" (LKN AA.05.0070) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Haut" (LKN AA.05.0080) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Muskulatur" (LKN AA.05.0090) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Gelenke" (LKN AA.05.0100) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Gefässe" (LKN AA.05.0110) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Lymphatische Organe" (LKN AA.05.0120) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Neurologie" (LKN AA.05.0130) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Pubertätsentwicklung" (LKN AA.05.0140) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Ärztliche, telemedizinische zeitgleiche Konsultation, erste 5 Min." (LKN AA.10.0010) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Mit welcher Tarifposition darf die Leistung AA.10.0010 nicht kumuliert werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „+ Ärztliche, telemedizinische zeitgleiche Konsultation, jede weitere 1 Min." (LKN AA.10.0020) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Wie oft darf die Leistung „Ärztliche, telemedizinische zeitversetzte Konsultation" (LKN AA.10.0030) pro tag abgerechnet werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Ärztliche, telemedizinische zeitversetzte Konsultation" (LKN AA.10.0030) pro tage abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Mit welcher Tarifposition darf die Leistung AA.10.0030 nicht kumuliert werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Ärztliches Expertenboard in An- oder Abwesenheit des Patienten, pro 1 Min." (LKN AA.15.0050) pro tage abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Mit welcher Tarifposition darf die Leistung AA.15.0090 nicht kumuliert werden?</t>
   </si>
   <si>
     <t>Mit welcher Tarifposition darf die Leistung AA.20.0010 nicht kumuliert werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Regionalanästhesie durch den Nichtanästhesisten (Operateur)" (LKN AA.20.0020) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Mit welcher Tarifposition darf die Leistung AA.20.0020 nicht kumuliert werden?</t>
   </si>
   <si>
     <t>Mit welcher Tarifposition darf die Leistung AA.20.0030 nicht kumuliert werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Stomapflege ohne Irrigation" (LKN AA.20.0040) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Stomapflege mit Irrigation" (LKN AA.20.0050) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Mit welcher Tarifposition darf die Leistung AA.20.0070 nicht kumuliert werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Erstellung eines ärztlichen Berichts zuhanden eines anderen Arztes, eines Therapeuten oder der Pflege, pro 1 Min." (LKN AA.25.0010) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Mit welcher Tarifposition darf die Leistung AA.25.0010 nicht kumuliert werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Erstellung eines ärztlichen Berichts zuhanden des Patienten oder eines Angehörigen, pro 1 Min." (LKN AA.25.0020) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Mit welcher Tarifposition darf die Leistung AA.25.0020 nicht kumuliert werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Erstellung eines ärztlichen Berichts zuhanden des Versicherers, pro 1 Min." (LKN AA.25.0030) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Mit welcher Tarifposition darf die Leistung AA.25.0030 nicht kumuliert werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Erstellung eines ärztlichen Zeugnisses in Abwesenheit des Patienten" (LKN AA.25.0040) pro sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>A) Einzelleistungstarif für ambulante ärztliche Leistungen in der Schweiz</t>
   </si>
   <si>
@@ -889,66 +784,27 @@
     <t>Im Leistungskatalog (z.B. TARDOC/AMBULANT), direkt neben dem Pauschalencode</t>
   </si>
   <si>
-    <t>Beliebig oft pro sitzung</t>
-  </si>
-  <si>
     <t>AA.20.0040</t>
   </si>
   <si>
-    <t>Maximal 30 mal pro sitzung</t>
-  </si>
-  <si>
-    <t>Maximal 2 mal pro sitzung</t>
-  </si>
-  <si>
     <t>CA.15.0070</t>
   </si>
   <si>
-    <t>Maximal 60 mal pro sitzung</t>
-  </si>
-  <si>
-    <t>Maximal 120 mal pro tage</t>
-  </si>
-  <si>
-    <t>Beliebig oft pro tage</t>
-  </si>
-  <si>
     <t>AA.00.0010</t>
   </si>
   <si>
-    <t>Maximal 20 mal pro tage</t>
-  </si>
-  <si>
     <t>AA.05.0030</t>
   </si>
   <si>
-    <t>Maximal 3 mal pro sitzung</t>
-  </si>
-  <si>
-    <t>Maximal 5 mal pro sitzung</t>
-  </si>
-  <si>
-    <t>Maximal 1 mal pro sitzung</t>
-  </si>
-  <si>
     <t>AA.05.0130</t>
   </si>
   <si>
-    <t>Maximal 15 mal pro sitzung</t>
-  </si>
-  <si>
     <t>Maximal 2 mal pro tag</t>
   </si>
   <si>
-    <t>Maximal 4 mal pro tage</t>
-  </si>
-  <si>
     <t>EA</t>
   </si>
   <si>
-    <t>Maximal 30 mal pro tage</t>
-  </si>
-  <si>
     <t>AA.25.0030</t>
   </si>
   <si>
@@ -967,12 +823,6 @@
     <t>AA.30.0090</t>
   </si>
   <si>
-    <t>Maximal 40 mal pro sitzung</t>
-  </si>
-  <si>
-    <t>Maximal 20 mal pro sitzung</t>
-  </si>
-  <si>
     <t>AA.20.0070</t>
   </si>
   <si>
@@ -1168,12 +1018,6 @@
     <t>AA.10.0010</t>
   </si>
   <si>
-    <t>Maximal 60 mal pro tage</t>
-  </si>
-  <si>
-    <t>Maximal 240 mal pro tage</t>
-  </si>
-  <si>
     <t>CG.00.0020</t>
   </si>
   <si>
@@ -1183,9 +1027,6 @@
     <t>Maximal 1 mal pro tag</t>
   </si>
   <si>
-    <t>Maximal 6 mal pro tage</t>
-  </si>
-  <si>
     <t>AA.05.0070</t>
   </si>
   <si>
@@ -1399,15 +1240,9 @@
     <t>AA.25.0010</t>
   </si>
   <si>
-    <t>Maximal 120 mal pro sitzung</t>
-  </si>
-  <si>
     <t>CA.15.0100</t>
   </si>
   <si>
-    <t>Maximal 40 mal pro tage</t>
-  </si>
-  <si>
     <t>AA.05</t>
   </si>
   <si>
@@ -1439,6 +1274,177 @@
   </si>
   <si>
     <t>Kumulation Konsultation und Telemedizin</t>
+  </si>
+  <si>
+    <t>Maximal 2 mal pro Sitzung</t>
+  </si>
+  <si>
+    <t>Maximal 1 mal pro Sitzung</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Ärztliche Konsultation, erste 5 Min." (LKN AA.00.0010) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Maximal 3 mal pro Sitzung</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „+ Ärztliche Konsultation, jede weitere 1 Min." (LKN AA.00.0020) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Maximal 30 mal pro Sitzung</t>
+  </si>
+  <si>
+    <t>Maximal 15 mal pro Sitzung</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Besuch, erste 5 Min." (LKN AA.00.0030) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „+ Besuch, jede weitere 1 Min." (LKN AA.00.0040) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Wegzeit, pro 1 Min." (LKN AA.00.0050) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Maximal 60 mal pro Sitzung</t>
+  </si>
+  <si>
+    <t>Maximal 120 mal pro Sitzung</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Instruktion von Selbstmessungen und/oder Selbstbehandlungen durch den Arzt, pro 1 Min." (LKN AA.00.0070) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Kreislauf" (LKN AA.05.0010) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Maximal 5 mal pro Sitzung</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Augen" (LKN AA.05.0020) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Ohren" (LKN AA.05.0030) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Luftwege" (LKN AA.05.0040) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Wirbelsäule" (LKN AA.05.0050) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Abdomen" (LKN AA.05.0060) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Uro-Genital" (LKN AA.05.0070) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Haut" (LKN AA.05.0080) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Muskulatur" (LKN AA.05.0090) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Gelenke" (LKN AA.05.0100) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Gefässe" (LKN AA.05.0110) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Lymphatische Organe" (LKN AA.05.0120) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Neurologie" (LKN AA.05.0130) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Pubertätsentwicklung" (LKN AA.05.0140) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Ärztliche, telemedizinische zeitgleiche Konsultation, erste 5 Min." (LKN AA.10.0010) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „+ Ärztliche, telemedizinische zeitgleiche Konsultation, jede weitere 1 Min." (LKN AA.10.0020) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Regionalanästhesie durch den Nichtanästhesisten (Operateur)" (LKN AA.20.0020) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Stomapflege ohne Irrigation" (LKN AA.20.0040) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Stomapflege mit Irrigation" (LKN AA.20.0050) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Erstellung eines ärztlichen Berichts zuhanden eines anderen Arztes, eines Therapeuten oder der Pflege, pro 1 Min." (LKN AA.25.0010) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Maximal 40 mal pro Sitzung</t>
+  </si>
+  <si>
+    <t>Maximal 20 mal pro Sitzung</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Erstellung eines ärztlichen Berichts zuhanden des Patienten oder eines Angehörigen, pro 1 Min." (LKN AA.25.0020) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Erstellung eines ärztlichen Berichts zuhanden des Versicherers, pro 1 Min." (LKN AA.25.0030) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Erstellung eines ärztlichen Zeugnisses in Abwesenheit des Patienten" (LKN AA.25.0040) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Vor-und Nachbesprechung diagnostischer/therapeutischer Eingriffe mit Patienten, pro 1 Min." (LKN AA.00.0060) pro Tage abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Maximal 120 mal pro Tage</t>
+  </si>
+  <si>
+    <t>Maximal 60 mal pro Tage</t>
+  </si>
+  <si>
+    <t>Beliebig oft pro Tage</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Instruktion von Selbstmessungen und/oder Selbstbehandlungen durch den Arzt, pro 1 Min." (LKN AA.00.0070) pro Tage abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Maximal 30 mal pro Tage</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Ärztliches Konsilium, pro 1 Min." (LKN AA.00.0080) pro Tage abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Maximal 240 mal pro Tage</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Spezifische lmpfberatung bei franchisebefreiten lmpfungen, pro 1 Min." (LKN AA.00.0090) pro Tage abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Maximal 20 mal pro Tage</t>
+  </si>
+  <si>
+    <t>Maximal 40 mal pro Tage</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Ärztliche, telemedizinische zeitversetzte Konsultation" (LKN AA.10.0030) pro Tage abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Maximal 4 mal pro Tage</t>
+  </si>
+  <si>
+    <t>Maximal 6 mal pro Tage</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Ärztliches Expertenboard in An- oder Abwesenheit des Patienten, pro 1 Min." (LKN AA.15.0050) pro Tage abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Maximal 120 mal pro 90 Tage</t>
+  </si>
+  <si>
+    <t>Maximal 60 mal pro 90 Tage</t>
+  </si>
+  <si>
+    <t>Beliebig oft pro 90 Tage</t>
   </si>
 </sst>
 </file>
@@ -1512,6 +1518,38 @@
       <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1540,38 +1578,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1586,15 +1592,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0DD1CE48-A2CB-4825-BA86-CF8BB2FE3479}" name="Tabelle1" displayName="Tabelle1" ref="A1:F116" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0DD1CE48-A2CB-4825-BA86-CF8BB2FE3479}" name="Tabelle1" displayName="Tabelle1" ref="A1:F116" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
   <autoFilter ref="A1:F116" xr:uid="{0DD1CE48-A2CB-4825-BA86-CF8BB2FE3479}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{FC806AA3-9713-4D9A-B8EC-BE6F97E4E7BA}" name="Stichwort" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{3B045A7F-F364-486C-A8F1-3FF822572156}" name="Frage" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{A0A5D70C-9389-400E-BCD2-FA8216077CAE}" name="Antwort_1" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{B8F64D72-999E-4FD4-9A25-C32A233F32BF}" name="Antwort_2" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{11EBCAFF-3D9F-426B-80D6-C66B8EB93DB2}" name="Antwort_3" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{84AC801A-DFAB-43FF-BC27-29777962FA50}" name="Korrekte_Antwort" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{FC806AA3-9713-4D9A-B8EC-BE6F97E4E7BA}" name="Stichwort" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{3B045A7F-F364-486C-A8F1-3FF822572156}" name="Frage" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{A0A5D70C-9389-400E-BCD2-FA8216077CAE}" name="Antwort_1" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{B8F64D72-999E-4FD4-9A25-C32A233F32BF}" name="Antwort_2" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{11EBCAFF-3D9F-426B-80D6-C66B8EB93DB2}" name="Antwort_3" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{84AC801A-DFAB-43FF-BC27-29777962FA50}" name="Korrekte_Antwort" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1889,19 +1895,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="E61" sqref="E60:E61"/>
+    <sheetView tabSelected="1" topLeftCell="B66" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.9375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.9296875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="39.234375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.3515625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.9375" style="2"/>
+    <col min="2" max="5" width="39.19921875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.9296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1921,7 +1927,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1929,19 +1935,19 @@
         <v>111</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>226</v>
+        <v>191</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>394</v>
+        <v>341</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1949,19 +1955,19 @@
         <v>112</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>227</v>
+        <v>192</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>319</v>
+        <v>269</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>395</v>
+        <v>342</v>
       </c>
       <c r="F3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1969,19 +1975,19 @@
         <v>113</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>228</v>
+        <v>193</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>320</v>
+        <v>270</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>396</v>
+        <v>343</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1989,19 +1995,19 @@
         <v>114</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>229</v>
+        <v>194</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>321</v>
+        <v>271</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>397</v>
+        <v>344</v>
       </c>
       <c r="F5" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2009,19 +2015,19 @@
         <v>115</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>230</v>
+        <v>195</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>398</v>
+        <v>345</v>
       </c>
       <c r="F6" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -2029,19 +2035,19 @@
         <v>116</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>231</v>
+        <v>196</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>323</v>
+        <v>273</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>399</v>
+        <v>346</v>
       </c>
       <c r="F7" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -2049,19 +2055,19 @@
         <v>117</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>232</v>
+        <v>197</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>400</v>
+        <v>347</v>
       </c>
       <c r="F8" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -2069,19 +2075,19 @@
         <v>118</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>233</v>
+        <v>198</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>325</v>
+        <v>275</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>401</v>
+        <v>348</v>
       </c>
       <c r="F9" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -2089,19 +2095,19 @@
         <v>119</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>326</v>
+        <v>276</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>402</v>
+        <v>349</v>
       </c>
       <c r="F10" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -2109,19 +2115,19 @@
         <v>120</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>327</v>
+        <v>277</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>403</v>
+        <v>350</v>
       </c>
       <c r="F11" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -2129,19 +2135,19 @@
         <v>121</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>328</v>
+        <v>278</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>404</v>
+        <v>351</v>
       </c>
       <c r="F12" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -2149,19 +2155,19 @@
         <v>122</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>329</v>
+        <v>279</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>405</v>
+        <v>352</v>
       </c>
       <c r="F13" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="100.35" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -2169,19 +2175,19 @@
         <v>123</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>238</v>
+        <v>203</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>330</v>
+        <v>280</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>406</v>
+        <v>353</v>
       </c>
       <c r="F14" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -2189,19 +2195,19 @@
         <v>124</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>331</v>
+        <v>281</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>407</v>
+        <v>354</v>
       </c>
       <c r="F15" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -2209,19 +2215,19 @@
         <v>125</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>408</v>
+        <v>355</v>
       </c>
       <c r="F16" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -2229,19 +2235,19 @@
         <v>126</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>241</v>
+        <v>206</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>333</v>
+        <v>283</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>409</v>
+        <v>356</v>
       </c>
       <c r="F17" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -2249,19 +2255,19 @@
         <v>127</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>334</v>
+        <v>284</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>410</v>
+        <v>357</v>
       </c>
       <c r="F18" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -2269,19 +2275,19 @@
         <v>128</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>335</v>
+        <v>285</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>411</v>
+        <v>358</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -2289,19 +2295,19 @@
         <v>129</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>336</v>
+        <v>286</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>412</v>
+        <v>359</v>
       </c>
       <c r="F20" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -2309,19 +2315,19 @@
         <v>130</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>337</v>
+        <v>287</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>413</v>
+        <v>360</v>
       </c>
       <c r="F21" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -2329,19 +2335,19 @@
         <v>131</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>338</v>
+        <v>288</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>414</v>
+        <v>361</v>
       </c>
       <c r="F22" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -2349,19 +2355,19 @@
         <v>132</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>339</v>
+        <v>289</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>415</v>
+        <v>362</v>
       </c>
       <c r="F23" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -2369,19 +2375,19 @@
         <v>133</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>340</v>
+        <v>290</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>416</v>
+        <v>363</v>
       </c>
       <c r="F24" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -2389,19 +2395,19 @@
         <v>134</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>341</v>
+        <v>291</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>417</v>
+        <v>364</v>
       </c>
       <c r="F25" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -2409,19 +2415,19 @@
         <v>135</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>342</v>
+        <v>292</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>418</v>
+        <v>365</v>
       </c>
       <c r="F26" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -2429,19 +2435,19 @@
         <v>136</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>343</v>
+        <v>293</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>419</v>
+        <v>366</v>
       </c>
       <c r="F27" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -2449,19 +2455,19 @@
         <v>137</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>344</v>
+        <v>294</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>420</v>
+        <v>367</v>
       </c>
       <c r="F28" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -2469,19 +2475,19 @@
         <v>138</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>345</v>
+        <v>295</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>421</v>
+        <v>368</v>
       </c>
       <c r="F29" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -2489,19 +2495,19 @@
         <v>139</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>254</v>
+        <v>219</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>346</v>
+        <v>296</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>422</v>
+        <v>369</v>
       </c>
       <c r="F30" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -2509,19 +2515,19 @@
         <v>140</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>347</v>
+        <v>297</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>423</v>
+        <v>370</v>
       </c>
       <c r="F31" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -2529,19 +2535,19 @@
         <v>141</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>348</v>
+        <v>298</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>424</v>
+        <v>371</v>
       </c>
       <c r="F32" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -2549,39 +2555,39 @@
         <v>142</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>349</v>
+        <v>299</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>425</v>
+        <v>372</v>
       </c>
       <c r="F33" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
-        <v>470</v>
+        <v>415</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>143</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>258</v>
+        <v>223</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>426</v>
+        <v>373</v>
       </c>
       <c r="F34" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
@@ -2589,39 +2595,39 @@
         <v>144</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>351</v>
+        <v>301</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>427</v>
+        <v>374</v>
       </c>
       <c r="F35" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
-        <v>471</v>
+        <v>416</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>145</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>352</v>
+        <v>302</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>428</v>
+        <v>375</v>
       </c>
       <c r="F36" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>38</v>
       </c>
@@ -2629,39 +2635,39 @@
         <v>146</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>353</v>
+        <v>303</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>429</v>
+        <v>376</v>
       </c>
       <c r="F37" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
-        <v>472</v>
+        <v>417</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>147</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>262</v>
+        <v>227</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>349</v>
+        <v>299</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>430</v>
+        <v>377</v>
       </c>
       <c r="F38" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
@@ -2669,19 +2675,19 @@
         <v>148</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>431</v>
+        <v>378</v>
       </c>
       <c r="F39" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
@@ -2689,19 +2695,19 @@
         <v>149</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>355</v>
+        <v>305</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>432</v>
+        <v>379</v>
       </c>
       <c r="F40" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
@@ -2709,19 +2715,19 @@
         <v>150</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>356</v>
+        <v>306</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>433</v>
+        <v>380</v>
       </c>
       <c r="F41" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
@@ -2729,19 +2735,19 @@
         <v>151</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>265</v>
+        <v>230</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>357</v>
+        <v>307</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>434</v>
+        <v>381</v>
       </c>
       <c r="F42" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>40</v>
       </c>
@@ -2749,19 +2755,19 @@
         <v>152</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>358</v>
+        <v>308</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>435</v>
+        <v>382</v>
       </c>
       <c r="F43" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>41</v>
       </c>
@@ -2769,19 +2775,19 @@
         <v>153</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>359</v>
+        <v>309</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>436</v>
+        <v>383</v>
       </c>
       <c r="F44" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>49</v>
       </c>
@@ -2789,19 +2795,19 @@
         <v>154</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>360</v>
+        <v>310</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>437</v>
+        <v>384</v>
       </c>
       <c r="F45" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>42</v>
       </c>
@@ -2809,19 +2815,19 @@
         <v>155</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>268</v>
+        <v>233</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>361</v>
+        <v>311</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>438</v>
+        <v>385</v>
       </c>
       <c r="F46" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>43</v>
       </c>
@@ -2829,19 +2835,19 @@
         <v>156</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>269</v>
+        <v>234</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>362</v>
+        <v>312</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>439</v>
+        <v>386</v>
       </c>
       <c r="F47" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
         <v>44</v>
       </c>
@@ -2849,19 +2855,19 @@
         <v>157</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>270</v>
+        <v>235</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>363</v>
+        <v>313</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>440</v>
+        <v>387</v>
       </c>
       <c r="F48" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>45</v>
       </c>
@@ -2869,19 +2875,19 @@
         <v>158</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>271</v>
+        <v>236</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>364</v>
+        <v>314</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>441</v>
+        <v>388</v>
       </c>
       <c r="F49" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>46</v>
       </c>
@@ -2889,19 +2895,19 @@
         <v>159</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>272</v>
+        <v>237</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>442</v>
+        <v>389</v>
       </c>
       <c r="F50" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
         <v>47</v>
       </c>
@@ -2909,19 +2915,19 @@
         <v>160</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>366</v>
+        <v>316</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>443</v>
+        <v>390</v>
       </c>
       <c r="F51" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>48</v>
       </c>
@@ -2929,19 +2935,19 @@
         <v>161</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>274</v>
+        <v>239</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>367</v>
+        <v>317</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>444</v>
+        <v>391</v>
       </c>
       <c r="F52" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>49</v>
       </c>
@@ -2949,19 +2955,19 @@
         <v>162</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>275</v>
+        <v>240</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>368</v>
+        <v>318</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>445</v>
+        <v>392</v>
       </c>
       <c r="F53" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
         <v>50</v>
       </c>
@@ -2969,19 +2975,19 @@
         <v>163</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>276</v>
+        <v>241</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>369</v>
+        <v>319</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>446</v>
+        <v>393</v>
       </c>
       <c r="F54" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
         <v>51</v>
       </c>
@@ -2989,19 +2995,19 @@
         <v>164</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>277</v>
+        <v>242</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>370</v>
+        <v>320</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>447</v>
+        <v>394</v>
       </c>
       <c r="F55" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>52</v>
       </c>
@@ -3009,19 +3015,19 @@
         <v>165</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>371</v>
+        <v>321</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>448</v>
+        <v>395</v>
       </c>
       <c r="F56" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>53</v>
       </c>
@@ -3029,19 +3035,19 @@
         <v>166</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>279</v>
+        <v>244</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>372</v>
+        <v>322</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>449</v>
+        <v>396</v>
       </c>
       <c r="F57" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>54</v>
       </c>
@@ -3049,19 +3055,19 @@
         <v>167</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>373</v>
+        <v>323</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>450</v>
+        <v>397</v>
       </c>
       <c r="F58" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>55</v>
       </c>
@@ -3069,19 +3075,19 @@
         <v>168</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>374</v>
+        <v>324</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>451</v>
+        <v>398</v>
       </c>
       <c r="F59" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>56</v>
       </c>
@@ -3089,19 +3095,19 @@
         <v>169</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>375</v>
+        <v>325</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>452</v>
+        <v>399</v>
       </c>
       <c r="F60" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>57</v>
       </c>
@@ -3109,19 +3115,19 @@
         <v>170</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>376</v>
+        <v>326</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>453</v>
+        <v>400</v>
       </c>
       <c r="F61" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
         <v>58</v>
       </c>
@@ -3129,19 +3135,19 @@
         <v>171</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>377</v>
+        <v>327</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>447</v>
+        <v>394</v>
       </c>
       <c r="F62" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>59</v>
       </c>
@@ -3149,19 +3155,19 @@
         <v>172</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>378</v>
+        <v>328</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>454</v>
+        <v>401</v>
       </c>
       <c r="F63" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
         <v>60</v>
       </c>
@@ -3169,19 +3175,19 @@
         <v>173</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>379</v>
+        <v>329</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>455</v>
+        <v>402</v>
       </c>
       <c r="F64" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>61</v>
       </c>
@@ -3189,19 +3195,19 @@
         <v>174</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>287</v>
+        <v>252</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>377</v>
+        <v>327</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>447</v>
+        <v>394</v>
       </c>
       <c r="F65" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
         <v>62</v>
       </c>
@@ -3209,1013 +3215,1013 @@
         <v>175</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>288</v>
+        <v>253</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>380</v>
+        <v>330</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>456</v>
+        <v>403</v>
       </c>
       <c r="F66" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>176</v>
+        <v>420</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>300</v>
+        <v>421</v>
       </c>
       <c r="F67" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>314</v>
+        <v>266</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>457</v>
+        <v>404</v>
       </c>
       <c r="F68" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>178</v>
+        <v>422</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>291</v>
+        <v>423</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>304</v>
+        <v>424</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="F69" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>179</v>
+        <v>425</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="F70" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>381</v>
+        <v>331</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>458</v>
+        <v>405</v>
       </c>
       <c r="F71" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>181</v>
+        <v>426</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>291</v>
+        <v>423</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>304</v>
+        <v>424</v>
       </c>
       <c r="F72" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>182</v>
+        <v>427</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>294</v>
+        <v>428</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>459</v>
+        <v>429</v>
       </c>
       <c r="F73" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>183</v>
+        <v>457</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>295</v>
+        <v>472</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>382</v>
+        <v>473</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>296</v>
+        <v>474</v>
       </c>
       <c r="F74" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>184</v>
+        <v>430</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>291</v>
+        <v>423</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>304</v>
+        <v>424</v>
       </c>
       <c r="F75" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>185</v>
+        <v>461</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>296</v>
+        <v>460</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>308</v>
+        <v>462</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>382</v>
+        <v>459</v>
       </c>
       <c r="F76" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>186</v>
+        <v>463</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>296</v>
+        <v>460</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>383</v>
+        <v>464</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>295</v>
+        <v>458</v>
       </c>
       <c r="F77" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>297</v>
+        <v>256</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>303</v>
+        <v>258</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>460</v>
+        <v>406</v>
       </c>
       <c r="F78" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>188</v>
+        <v>465</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>298</v>
+        <v>466</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>296</v>
+        <v>460</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="F79" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>299</v>
+        <v>257</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>384</v>
+        <v>332</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>460</v>
+        <v>406</v>
       </c>
       <c r="F80" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>190</v>
+        <v>431</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>301</v>
+        <v>432</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="F81" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>191</v>
+        <v>433</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="F82" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A83" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>192</v>
+        <v>434</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>300</v>
+        <v>421</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="F83" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A84" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>193</v>
+        <v>435</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>301</v>
+        <v>432</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="F84" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A85" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>194</v>
+        <v>436</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>300</v>
+        <v>421</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="F85" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A86" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>195</v>
+        <v>437</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>301</v>
+        <v>432</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="F86" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A87" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>196</v>
+        <v>438</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="F87" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A88" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>197</v>
+        <v>439</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>300</v>
+        <v>421</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="F88" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A89" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>198</v>
+        <v>440</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="F89" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A90" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>199</v>
+        <v>441</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="F90" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A91" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>200</v>
+        <v>442</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>301</v>
+        <v>432</v>
       </c>
       <c r="F91" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A92" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>201</v>
+        <v>443</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="F92" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A93" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>202</v>
+        <v>444</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>292</v>
+        <v>418</v>
       </c>
       <c r="F93" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A94" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>203</v>
+        <v>445</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>301</v>
+        <v>432</v>
       </c>
       <c r="F94" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A95" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>204</v>
+        <v>446</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>301</v>
+        <v>432</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="F95" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A96" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>303</v>
+        <v>258</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>385</v>
+        <v>333</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>462</v>
+        <v>407</v>
       </c>
       <c r="F96" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A97" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>206</v>
+        <v>447</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>304</v>
+        <v>424</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>291</v>
+        <v>423</v>
       </c>
       <c r="F97" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A98" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>305</v>
+        <v>259</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>386</v>
+        <v>334</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>463</v>
+        <v>408</v>
       </c>
       <c r="F98" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A99" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>208</v>
+        <v>468</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>306</v>
+        <v>469</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>387</v>
+        <v>470</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>296</v>
+        <v>460</v>
       </c>
       <c r="F99" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A100" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>307</v>
+        <v>260</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>388</v>
+        <v>335</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>464</v>
+        <v>409</v>
       </c>
       <c r="F100" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A101" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>210</v>
+        <v>471</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>308</v>
+        <v>462</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>382</v>
+        <v>459</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>296</v>
+        <v>460</v>
       </c>
       <c r="F101" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A102" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>309</v>
+        <v>261</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>389</v>
+        <v>336</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>465</v>
+        <v>410</v>
       </c>
       <c r="F102" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A103" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>310</v>
+        <v>262</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>390</v>
+        <v>337</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>466</v>
+        <v>411</v>
       </c>
       <c r="F103" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A104" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>213</v>
+        <v>448</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>300</v>
+        <v>421</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="F104" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A105" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>311</v>
+        <v>263</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>390</v>
+        <v>337</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>467</v>
+        <v>412</v>
       </c>
       <c r="F105" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A106" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>215</v>
+        <v>186</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>312</v>
+        <v>264</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>391</v>
+        <v>338</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>468</v>
+        <v>413</v>
       </c>
       <c r="F106" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A107" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>216</v>
+        <v>449</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>300</v>
+        <v>421</v>
       </c>
       <c r="F107" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="43" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A108" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>217</v>
+        <v>450</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>300</v>
+        <v>421</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="F108" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A109" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>218</v>
+        <v>187</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>313</v>
+        <v>265</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>392</v>
+        <v>339</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>469</v>
+        <v>414</v>
       </c>
       <c r="F109" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A110" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>219</v>
+        <v>451</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>315</v>
+        <v>452</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>316</v>
+        <v>453</v>
       </c>
       <c r="F110" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A111" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>314</v>
+        <v>266</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>303</v>
+        <v>258</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>310</v>
+        <v>262</v>
       </c>
       <c r="F111" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A112" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>221</v>
+        <v>454</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>315</v>
+        <v>452</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>316</v>
+        <v>453</v>
       </c>
       <c r="F112" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A113" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>222</v>
+        <v>189</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>309</v>
+        <v>261</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>311</v>
+        <v>263</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>460</v>
+        <v>406</v>
       </c>
       <c r="F113" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A114" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>223</v>
+        <v>455</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>316</v>
+        <v>453</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>315</v>
+        <v>452</v>
       </c>
       <c r="F114" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A115" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>393</v>
+        <v>340</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>469</v>
+        <v>414</v>
       </c>
       <c r="F115" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A116" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>225</v>
+        <v>456</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>301</v>
+        <v>432</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="F116" s="2">
         <v>2</v>

</xml_diff>

<commit_message>
In den Fragen "LKN" entfernt
</commit_message>
<xml_diff>
--- a/Neuer_Arzttarif_Frage_Antwort_Spiel.xlsx
+++ b/Neuer_Arzttarif_Frage_Antwort_Spiel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beata\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a5b72c7ff873d10/Dokumente/Private Projekte/Python/Brick/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CE71BB-370B-42D9-8304-EA8B518DDE03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{B5CE71BB-370B-42D9-8304-EA8B518DDE03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E30DCB11-43C1-4B56-897D-C2D3F3F31862}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="1785" windowWidth="36645" windowHeight="19815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="1065" windowWidth="36645" windowHeight="19815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1213,15 +1213,9 @@
     <t>Wie oft darf die Leistung „Ärztliche Konsultation, erste 5 Min." (AA.00.0010) pro Sitzung abgerechnet werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „+ Ärztliche Konsultation, jede weitere 1 Min." (LKN AA.00.0020) pro Sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Wie oft darf die Leistung „Besuch, erste 5 Min." (AA.00.0030) pro Sitzung abgerechnet werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „+ Besuch, jede weitere 1 Min." (LKN AA.00.0040) pro Sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Wie oft darf die Leistung „Wegzeit, pro 1 Min." (AA.00.0050) pro Sitzung abgerechnet werden?</t>
   </si>
   <si>
@@ -1237,12 +1231,6 @@
     <t>Maximal 120 pro 90 Tage</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Instruktion von Selbstmessungen und/oder Selbstbehandlungen durch den Arzt, pro 1 Min." (LKN AA.00.0070) pro Sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Instruktion von Selbstmessungen und/oder Selbstbehandlungen durch den Arzt, pro 1 Min." (LKN AA.00.0070) pro 90 Tage abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Maximal 15 pro 90 Tage</t>
   </si>
   <si>
@@ -1252,9 +1240,6 @@
     <t>Maximal 30 pro 90 Tage</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Ärztliches Konsilium, pro 1 Min." (LKN AA.00.0080) pro 180 Tage abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Maximal 120 pro 180 Tage</t>
   </si>
   <si>
@@ -1264,39 +1249,21 @@
     <t>Maximal 140 pro 180 Tage</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Spezifische lmpfberatung bei franchisebefreiten lmpfungen, pro 1 Min." (LKN AA.00.0090) pro 90 Tage abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Maximal 25 pro 90 Tage</t>
   </si>
   <si>
     <t>Maximal 40 pro 90 Tage</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Kreislauf" (LKN AA.05.0010) pro Sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Augen" (LKN AA.05.0020) pro Sitzung abgerechnet werden?</t>
-  </si>
-  <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Ohren" (LKN AA.05.0030) pro Sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Wie oft darf die Leistung „Untersuchung: Luftwege" (AA.05.0040) pro Sitzung abgerechnet werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Wirbelsäule" (LKN AA.05.0050) pro Sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Wie oft darf die Leistung „Untersuchung: Abdomen" (AA.05.0060) pro Sitzung abgerechnet werden?</t>
   </si>
   <si>
     <t>Wie oft darf die Leistung „Untersuchung: Uro-Genital" (AA.05.0070) pro Sitzung abgerechnet werden?</t>
   </si>
   <si>
-    <t>Wie oft darf die Leistung „Untersuchung: Haut" (LKN AA.05.0080) pro Sitzung abgerechnet werden?</t>
-  </si>
-  <si>
     <t>Wie oft darf die Leistung „Untersuchung: Muskulatur" (AA.05.0090 – Untersuchung: Muskulatur) pro Sitzung abgerechnet werden?</t>
   </si>
   <si>
@@ -1346,6 +1313,39 @@
   </si>
   <si>
     <t>Wie oft darf die Leistung „Erstellung eines ärztlichen Zeugnisses in Abwesenheit des Patienten" (AA.25.0040) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „+ Ärztliche Konsultation, jede weitere 1 Min." (AA.00.0020) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „+ Besuch, jede weitere 1 Min." (AA.00.0040) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Instruktion von Selbstmessungen und/oder Selbstbehandlungen durch den Arzt, pro 1 Min." (AA.00.0070) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Instruktion von Selbstmessungen und/oder Selbstbehandlungen durch den Arzt, pro 1 Min." (AA.00.0070) pro 90 Tage abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Ärztliches Konsilium, pro 1 Min." (AA.00.0080) pro 180 Tage abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Spezifische lmpfberatung bei franchisebefreiten lmpfungen, pro 1 Min." (AA.00.0090) pro 90 Tage abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Kreislauf" (AA.05.0010) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Augen" (AA.05.0020) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Ohren" (AA.05.0030) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Wirbelsäule" (AA.05.0050) pro Sitzung abgerechnet werden?</t>
+  </si>
+  <si>
+    <t>Wie oft darf die Leistung „Untersuchung: Haut" (AA.05.0080) pro Sitzung abgerechnet werden?</t>
   </si>
 </sst>
 </file>
@@ -1410,6 +1410,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1437,20 +1451,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1465,7 +1465,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D6FCFD1-7E2C-458C-A372-B6908948FCD8}" name="Tabelle1" displayName="Tabelle1" ref="A1:F112" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D6FCFD1-7E2C-458C-A372-B6908948FCD8}" name="Tabelle1" displayName="Tabelle1" ref="A1:F112" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:F112" xr:uid="{8D6FCFD1-7E2C-458C-A372-B6908948FCD8}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{0909127D-D28C-4B12-B595-3EE287B9D046}" name="Stichwort"/>
@@ -1767,7 +1767,7 @@
   <dimension ref="A1:F112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3142,7 +3142,7 @@
         <v>169</v>
       </c>
       <c r="B69" t="s">
-        <v>397</v>
+        <v>431</v>
       </c>
       <c r="C69" t="s">
         <v>170</v>
@@ -3162,7 +3162,7 @@
         <v>185</v>
       </c>
       <c r="B70" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C70" t="s">
         <v>157</v>
@@ -3202,7 +3202,7 @@
         <v>308</v>
       </c>
       <c r="B72" t="s">
-        <v>399</v>
+        <v>432</v>
       </c>
       <c r="C72" t="s">
         <v>170</v>
@@ -3222,7 +3222,7 @@
         <v>309</v>
       </c>
       <c r="B73" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C73" t="s">
         <v>310</v>
@@ -3242,16 +3242,16 @@
         <v>313</v>
       </c>
       <c r="B74" t="s">
+        <v>399</v>
+      </c>
+      <c r="C74" t="s">
+        <v>400</v>
+      </c>
+      <c r="D74" t="s">
         <v>401</v>
       </c>
-      <c r="C74" t="s">
+      <c r="E74" t="s">
         <v>402</v>
-      </c>
-      <c r="D74" t="s">
-        <v>403</v>
-      </c>
-      <c r="E74" t="s">
-        <v>404</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -3262,7 +3262,7 @@
         <v>314</v>
       </c>
       <c r="B75" t="s">
-        <v>405</v>
+        <v>433</v>
       </c>
       <c r="C75" t="s">
         <v>170</v>
@@ -3282,16 +3282,16 @@
         <v>314</v>
       </c>
       <c r="B76" t="s">
-        <v>406</v>
+        <v>434</v>
       </c>
       <c r="C76" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D76" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E76" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -3302,16 +3302,16 @@
         <v>315</v>
       </c>
       <c r="B77" t="s">
-        <v>410</v>
+        <v>435</v>
       </c>
       <c r="C77" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D77" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="E77" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -3342,16 +3342,16 @@
         <v>319</v>
       </c>
       <c r="B79" t="s">
-        <v>414</v>
+        <v>436</v>
       </c>
       <c r="C79" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D79" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="E79" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -3382,7 +3382,7 @@
         <v>325</v>
       </c>
       <c r="B81" t="s">
-        <v>417</v>
+        <v>437</v>
       </c>
       <c r="C81" t="s">
         <v>157</v>
@@ -3402,7 +3402,7 @@
         <v>326</v>
       </c>
       <c r="B82" t="s">
-        <v>418</v>
+        <v>438</v>
       </c>
       <c r="C82" t="s">
         <v>157</v>
@@ -3422,7 +3422,7 @@
         <v>327</v>
       </c>
       <c r="B83" t="s">
-        <v>419</v>
+        <v>439</v>
       </c>
       <c r="C83" t="s">
         <v>157</v>
@@ -3442,7 +3442,7 @@
         <v>328</v>
       </c>
       <c r="B84" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="C84" t="s">
         <v>157</v>
@@ -3462,7 +3462,7 @@
         <v>329</v>
       </c>
       <c r="B85" t="s">
-        <v>421</v>
+        <v>440</v>
       </c>
       <c r="C85" t="s">
         <v>157</v>
@@ -3482,7 +3482,7 @@
         <v>330</v>
       </c>
       <c r="B86" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="C86" t="s">
         <v>157</v>
@@ -3502,7 +3502,7 @@
         <v>331</v>
       </c>
       <c r="B87" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="C87" t="s">
         <v>157</v>
@@ -3522,7 +3522,7 @@
         <v>332</v>
       </c>
       <c r="B88" t="s">
-        <v>424</v>
+        <v>441</v>
       </c>
       <c r="C88" t="s">
         <v>157</v>
@@ -3542,7 +3542,7 @@
         <v>333</v>
       </c>
       <c r="B89" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="C89" t="s">
         <v>157</v>
@@ -3562,7 +3562,7 @@
         <v>334</v>
       </c>
       <c r="B90" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="C90" t="s">
         <v>157</v>
@@ -3582,7 +3582,7 @@
         <v>335</v>
       </c>
       <c r="B91" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="C91" t="s">
         <v>157</v>
@@ -3602,7 +3602,7 @@
         <v>336</v>
       </c>
       <c r="B92" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="C92" t="s">
         <v>157</v>
@@ -3622,7 +3622,7 @@
         <v>337</v>
       </c>
       <c r="B93" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="C93" t="s">
         <v>157</v>
@@ -3642,7 +3642,7 @@
         <v>338</v>
       </c>
       <c r="B94" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="C94" t="s">
         <v>157</v>
@@ -3662,7 +3662,7 @@
         <v>339</v>
       </c>
       <c r="B95" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="C95" t="s">
         <v>157</v>
@@ -3702,7 +3702,7 @@
         <v>343</v>
       </c>
       <c r="B97" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="C97" t="s">
         <v>170</v>
@@ -3722,7 +3722,7 @@
         <v>344</v>
       </c>
       <c r="B98" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="C98" t="s">
         <v>345</v>
@@ -3742,7 +3742,7 @@
         <v>344</v>
       </c>
       <c r="B99" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
       <c r="C99" t="s">
         <v>345</v>
@@ -3782,7 +3782,7 @@
         <v>353</v>
       </c>
       <c r="B101" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="C101" t="s">
         <v>172</v>
@@ -3822,7 +3822,7 @@
         <v>358</v>
       </c>
       <c r="B103" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="C103" t="s">
         <v>157</v>
@@ -3842,7 +3842,7 @@
         <v>359</v>
       </c>
       <c r="B104" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="C104" t="s">
         <v>157</v>
@@ -3882,7 +3882,7 @@
         <v>363</v>
       </c>
       <c r="B106" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="C106" t="s">
         <v>171</v>
@@ -3922,7 +3922,7 @@
         <v>368</v>
       </c>
       <c r="B108" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="C108" t="s">
         <v>171</v>
@@ -3962,7 +3962,7 @@
         <v>371</v>
       </c>
       <c r="B110" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="C110" t="s">
         <v>171</v>
@@ -4002,7 +4002,7 @@
         <v>377</v>
       </c>
       <c r="B112" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="C112" t="s">
         <v>157</v>

</xml_diff>